<commit_message>
Intro and Des finished
next step: assumption and model
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -16,12 +16,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>impact velocity</t>
   </si>
   <si>
     <t>residual velocity</t>
+  </si>
+  <si>
+    <t>Desity</t>
+  </si>
+  <si>
+    <t>Poisson ratio</t>
+  </si>
+  <si>
+    <t>Interlaminar shearstrength (MPa)</t>
+  </si>
+  <si>
+    <t>In-plane shear strength(MPa)</t>
+  </si>
+  <si>
+    <t>Young's modulus (GPa)</t>
+  </si>
+  <si>
+    <t>In-plane shear modulus(GPa)</t>
+  </si>
+  <si>
+    <t>Interlaminar shear modulus(GPa)</t>
+  </si>
+  <si>
+    <t>Tensile Strength(MPa)</t>
+  </si>
+  <si>
+    <t>Compressive strength(MPa)</t>
   </si>
 </sst>
 </file>
@@ -45,7 +72,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -53,12 +80,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -77,16 +120,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>209551</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>456628</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>170922</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>285751</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>140677</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -103,8 +146,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4095750" y="1276350"/>
-          <a:ext cx="4580953" cy="4228572"/>
+          <a:off x="2333626" y="304800"/>
+          <a:ext cx="3124200" cy="2883877"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -403,18 +446,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="J3" sqref="J3:K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="10" max="10" width="31.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -422,7 +466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>400</v>
       </c>
@@ -430,13 +474,69 @@
         <v>220</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>360</v>
       </c>
       <c r="B3">
         <v>183</v>
       </c>
+      <c r="J3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="1">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" s="1">
+        <v>10.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
composite structure almost finished
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>impact velocity</t>
   </si>
@@ -49,6 +49,12 @@
   </si>
   <si>
     <t>Compressive strength(MPa)</t>
+  </si>
+  <si>
+    <t>[0/90/0/90/45/-45]</t>
+  </si>
+  <si>
+    <t>stcking sequece</t>
   </si>
 </sst>
 </file>
@@ -446,15 +452,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3:K11"/>
+      <selection activeCell="B23" sqref="B23:C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="31.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -537,6 +545,14 @@
         <v>4</v>
       </c>
       <c r="K11" s="1"/>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>